<commit_message>
R and Julia repication getting_started
</commit_message>
<xml_diff>
--- a/Documents/State_of_Package.xlsx
+++ b/Documents/State_of_Package.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umcutrecht-my.sharepoint.com/personal/f_j_metwaly_umcutrecht_nl/Documents/Documenten/GitHub/thesis_TTE/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC1048FA699B42E05ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5769DF6-62F4-4D68-B62D-C9EAE04FC9E2}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_F25DC773A252ABDACC1048FA699B42E05ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3223D23A-4507-41FF-AA91-367F6C850C38}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5916" yWindow="2028" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Legend:</t>
   </si>
   <si>
-    <t xml:space="preserve">IPCW </t>
-  </si>
-  <si>
-    <t>IPTW</t>
-  </si>
-  <si>
     <t>artificial censoring</t>
   </si>
   <si>
@@ -79,6 +73,39 @@
   </si>
   <si>
     <t>Naïve Model</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>IPCW (outcome censoring)</t>
+  </si>
+  <si>
+    <t>Marginal Effect Estimation</t>
+  </si>
+  <si>
+    <t>IPTW (baseline)</t>
+  </si>
+  <si>
+    <t>IPTW (post baseline)</t>
+  </si>
+  <si>
+    <t>chose n control</t>
+  </si>
+  <si>
+    <t>chose n control with matching  on confounders</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>data generation</t>
+  </si>
+  <si>
+    <t>Vignette IPCW</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -101,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -179,6 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -194,6 +228,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="163" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,110 +508,166 @@
     <col min="5" max="5" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>